<commit_message>
Big Update 7.1 ReliableUDP und 4.2 Pünktlichkeitsassistent
</commit_message>
<xml_diff>
--- a/Blatt 4-6/NetworkPerformance6.1.xlsx
+++ b/Blatt 4-6/NetworkPerformance6.1.xlsx
@@ -186,10 +186,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -250,8 +250,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.21502958880590189"/>
-          <c:y val="2.7806654487252034E-2"/>
+          <c:x val="0.13669683405756855"/>
+          <c:y val="2.7806659976433248E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -289,25 +289,25 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="7.4620879397600412E-2"/>
-          <c:y val="0.1763673548574847"/>
-          <c:w val="0.91240258852030709"/>
-          <c:h val="0.70807549156065619"/>
+          <c:x val="0.13212431433622662"/>
+          <c:y val="0.11791989200152057"/>
+          <c:w val="0.77258070956898006"/>
+          <c:h val="0.80907077091535828"/>
         </c:manualLayout>
       </c:layout>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="4"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$D$1</c:f>
+              <c:f>Tabelle1!$B$1:$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TCP Senderate in kbit/s</c:v>
+                  <c:v>UDP Senderate in kbit/s UDP Empfangsrate in kbit/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -315,12 +315,12 @@
           <c:spPr>
             <a:ln w="22225" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst>
               <a:glow rad="139700">
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent5">
                   <a:satMod val="175000"/>
                   <a:alpha val="14000"/>
                 </a:schemeClr>
@@ -332,7 +332,7 @@
             <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1">
+                <a:schemeClr val="accent5">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
                 </a:schemeClr>
@@ -342,271 +342,7 @@
               </a:ln>
               <a:effectLst>
                 <a:glow rad="63500">
-                  <a:schemeClr val="accent1">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$D$3:$D$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>565.10400000000004</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>565.10400000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>565.10400000000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>565.10400000000004</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TCP Empfangsrate in kbit/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent2">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="lt1">
-                          <a:lumMod val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$E$3:$E$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>546.47799999999995</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>546.51</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>546.58000000000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>546.42999999999995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>UDP Senderate in kbit/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent3">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent3">
+                  <a:schemeClr val="accent5">
                     <a:satMod val="175000"/>
                     <a:alpha val="25000"/>
                   </a:schemeClr>
@@ -619,8 +355,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.3981748104796416E-2"/>
-                  <c:y val="4.4511583916705739E-2"/>
+                  <c:x val="9.2266741567460396E-4"/>
+                  <c:y val="-3.0779630737393496E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -640,8 +376,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.1198378211172462E-2"/>
-                  <c:y val="4.4511583916705739E-2"/>
+                  <c:x val="-4.8744349156582475E-3"/>
+                  <c:y val="-3.0779630737393544E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -661,8 +397,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.4062846675468392E-2"/>
-                  <c:y val="3.3384597351785637E-2"/>
+                  <c:x val="9.2266741567460396E-4"/>
+                  <c:y val="-3.5912768984527881E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -682,8 +418,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-4.9859949006801317E-2"/>
-                  <c:y val="3.0818028228218518E-2"/>
+                  <c:x val="4.7874023032298384E-3"/>
+                  <c:y val="-5.1139395017218009E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -737,6 +473,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -754,9 +491,9 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:val>
+          <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$B$3:$B$6</c:f>
+              <c:f>Tabelle1!$B$9:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
@@ -774,19 +511,40 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$9:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>547.22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>547.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>547.16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>547.32000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
+          <c:idx val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$C$1</c:f>
+              <c:f>Tabelle1!$D$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>UDP Empfangsrate in kbit/s</c:v>
+                  <c:v>TCP Senderate in kbit/s TCP Empfangsrate in kbit/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -794,12 +552,12 @@
           <c:spPr>
             <a:ln w="22225" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent1"/>
               </a:solidFill>
             </a:ln>
             <a:effectLst>
               <a:glow rad="139700">
-                <a:schemeClr val="accent4">
+                <a:schemeClr val="accent1">
                   <a:satMod val="175000"/>
                   <a:alpha val="14000"/>
                 </a:schemeClr>
@@ -811,7 +569,7 @@
             <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent4">
+                <a:schemeClr val="accent1">
                   <a:lumMod val="60000"/>
                   <a:lumOff val="40000"/>
                 </a:schemeClr>
@@ -821,7 +579,7 @@
               </a:ln>
               <a:effectLst>
                 <a:glow rad="63500">
-                  <a:schemeClr val="accent4">
+                  <a:schemeClr val="accent1">
                     <a:satMod val="175000"/>
                     <a:alpha val="25000"/>
                   </a:schemeClr>
@@ -834,8 +592,8 @@
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.8963222482897408E-2"/>
-                  <c:y val="4.9644722163840076E-2"/>
+                  <c:x val="6.1787068627497223E-3"/>
+                  <c:y val="-2.3079923366691995E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -855,8 +613,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.9814224932743794E-2"/>
-                  <c:y val="4.9858737652175224E-2"/>
+                  <c:x val="1.4449239522117923E-2"/>
+                  <c:y val="-2.8213061613826237E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -876,8 +634,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.9657048903655352E-2"/>
-                  <c:y val="5.3917150340322927E-2"/>
+                  <c:x val="1.0584504634562689E-2"/>
+                  <c:y val="-1.2813646872423326E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -897,8 +655,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.7724681459877736E-2"/>
-                  <c:y val="5.1350581216755765E-2"/>
+                  <c:x val="1.2516872078340289E-2"/>
+                  <c:y val="-7.6805086252890861E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -952,6 +710,7 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -969,28 +728,49 @@
               </c:ext>
             </c:extLst>
           </c:dLbls>
-          <c:val>
+          <c:xVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$3:$C$6</c:f>
+              <c:f>Tabelle1!$E$9:$E$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>546.57000000000005</c:v>
+                  <c:v>547.23</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>546.59</c:v>
+                  <c:v>547.14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>546.54</c:v>
+                  <c:v>547.35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>546.52</c:v>
+                  <c:v>547.32000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$E$3:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>546.47799999999995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>546.51</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>546.58000000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>546.42999999999995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:dLblPos val="t"/>
@@ -1001,13 +781,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1066175568"/>
-        <c:axId val="1066176112"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1066175568"/>
+        <c:axId val="63544704"/>
+        <c:axId val="2042873424"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="63544704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1058,7 +836,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE" sz="1050"/>
-                  <a:t>Messungen</a:t>
+                  <a:t>UDP/TCP Senderate in kbit/s</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1092,6 +870,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1121,15 +900,13 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1066176112"/>
+        <c:crossAx val="2042873424"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1066176112"/>
+        <c:axId val="2042873424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1178,6 +955,14 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1050"/>
+                  <a:t>UDP/TCP Empfangsrate</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1050" baseline="0"/>
+                  <a:t> in </a:t>
+                </a:r>
                 <a:r>
                   <a:rPr lang="de-DE" sz="1050"/>
                   <a:t>kbit/s</a:t>
@@ -1244,10 +1029,10 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1066175568"/>
+        <c:crossAx val="63544704"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="2"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1259,7 +1044,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13083133754888951"/>
+          <c:y val="7.7806712627798036E-2"/>
+          <c:w val="0.86916863607816652"/>
+          <c:h val="4.5135698362437256E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1367,7 +1161,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13669683405756855"/>
+          <c:y val="2.7806659976433248E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1398,20 +1199,266 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13212431433622662"/>
+          <c:y val="0.11791989200152057"/>
+          <c:w val="0.77258070956898006"/>
+          <c:h val="0.80907077091535828"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="4"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Tabelle1!$D$1</c:f>
+              <c:f>Tabelle1!$B$1:$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>TCP Senderate in kbit/s</c:v>
+                  <c:v>UDP Senderate in kbit/s UDP Empfangsrate in kbit/s</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent5">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.2266741567460396E-4"/>
+                  <c:y val="-3.0779630737393496E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-4.8744349156582475E-3"/>
+                  <c:y val="-3.0779630737393544E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="9.2266741567460396E-4"/>
+                  <c:y val="-3.5912768984527881E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="4.7874023032298384E-3"/>
+                  <c:y val="-5.1139395017218009E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$B$9:$B$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>565.10400000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>565.10400000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>565.10400000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>565.10400000000004</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$9:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>547.22</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>547.12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>547.16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>547.32000000000005</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$D$1:$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>TCP Senderate in kbit/s TCP Empfangsrate in kbit/s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1454,82 +1501,147 @@
               </a:effectLst>
             </c:spPr>
           </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$D$9:$D$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>565.10400000000004</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>565.10400000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>565.10400000000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>565.10400000000004</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>TCP Empfangsrate in kbit/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent2">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="4"/>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="6.1787068627497223E-3"/>
+                  <c:y val="-2.3079923366691995E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.4449239522117923E-2"/>
+                  <c:y val="-2.8213061613826237E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.0584504634562689E-2"/>
+                  <c:y val="-1.2813646872423326E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.2516872078340289E-2"/>
+                  <c:y val="-7.6805086252890861E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln>
                 <a:noFill/>
               </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent2">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
+              <a:effectLst/>
             </c:spPr>
-          </c:marker>
-          <c:val>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
             <c:numRef>
               <c:f>Tabelle1!$E$9:$E$12</c:f>
               <c:numCache>
@@ -1549,174 +1661,44 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>UDP Empfangsrate in kbit/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent3">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent3">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
-            </c:spPr>
-          </c:marker>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Tabelle1!$C$9:$C$12</c:f>
+              <c:f>Tabelle1!$E$3:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>547.22</c:v>
+                  <c:v>546.47799999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>547.12</c:v>
+                  <c:v>546.51</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>547.16</c:v>
+                  <c:v>546.58000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>547.32000000000005</c:v>
+                  <c:v>546.42999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Tabelle1!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>UDP Senderate in kbit/s</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="22225" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-            </a:ln>
-            <a:effectLst>
-              <a:glow rad="139700">
-                <a:schemeClr val="accent4">
-                  <a:satMod val="175000"/>
-                  <a:alpha val="14000"/>
-                </a:schemeClr>
-              </a:glow>
-            </a:effectLst>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="4"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst>
-                <a:glow rad="63500">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="175000"/>
-                    <a:alpha val="25000"/>
-                  </a:schemeClr>
-                </a:glow>
-              </a:effectLst>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>Tabelle1!$B$9:$B$12</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>565.10400000000004</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>565.10400000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>565.10400000000004</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>565.10400000000004</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1070720304"/>
-        <c:axId val="1070718672"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1070720304"/>
+        <c:axId val="67788912"/>
+        <c:axId val="67793808"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="67788912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1754,7 +1736,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="lt1">
                         <a:lumMod val="75000"/>
@@ -1766,138 +1748,8 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-DE" sz="1000"/>
-                  <a:t>Messungen</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout>
-            <c:manualLayout>
-              <c:xMode val="edge"/>
-              <c:yMode val="edge"/>
-              <c:x val="0.48246162988697533"/>
-              <c:y val="0.94066463495568697"/>
-            </c:manualLayout>
-          </c:layout>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="lt1">
-                      <a:lumMod val="75000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="de-DE"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="lt1">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1070718672"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1070718672"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="536"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:gradFill>
-                <a:gsLst>
-                  <a:gs pos="100000">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="75000"/>
-                      <a:lumOff val="25000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                  <a:gs pos="0">
-                    <a:schemeClr val="dk1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:gs>
-                </a:gsLst>
-                <a:lin ang="5400000" scaled="0"/>
-              </a:gradFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="lt1">
-                        <a:lumMod val="75000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="de-DE" sz="1000"/>
-                  <a:t>kbit/s</a:t>
+                  <a:rPr lang="de-DE" sz="1050"/>
+                  <a:t>UDP/TCP Senderate in kbit/s</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1912,11 +1764,11 @@
             <a:effectLst/>
           </c:spPr>
           <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="lt1">
                       <a:lumMod val="75000"/>
@@ -1961,10 +1813,139 @@
             <a:endParaRPr lang="de-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1070720304"/>
+        <c:crossAx val="67793808"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="2"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="67793808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1050"/>
+                  <a:t>UDP/TCP Empfangsrate</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1050" baseline="0"/>
+                  <a:t> in </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-DE" sz="1050"/>
+                  <a:t>kbit/s</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1050" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="67788912"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="5.000000000000001E-2"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1976,7 +1957,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13083133754888951"/>
+          <c:y val="7.7806712627798036E-2"/>
+          <c:w val="0.86916863607816652"/>
+          <c:h val="4.5135698362437256E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3228,15 +3218,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:colOff>66675</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>71436</xdr:rowOff>
+      <xdr:rowOff>90485</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1142999</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>66676</xdr:rowOff>
+      <xdr:colOff>1504950</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3257,21 +3247,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1190625</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>71436</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1543050</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1524000</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>100015</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Diagramm 5"/>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvPr id="5" name="Diagramm 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -3553,8 +3545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3566,8 +3558,8 @@
     <col min="6" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" customWidth="1"/>
     <col min="12" max="12" width="28" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.140625" customWidth="1"/>
   </cols>
@@ -3606,18 +3598,18 @@
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
     </row>
@@ -3804,18 +3796,18 @@
       <c r="L7" s="5"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
@@ -3832,7 +3824,7 @@
       <c r="D9" s="1">
         <v>565.10400000000004</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="9">
         <v>547.23</v>
       </c>
       <c r="F9" s="1">
@@ -3874,7 +3866,7 @@
       <c r="D10" s="1">
         <v>565.10400000000004</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>547.14</v>
       </c>
       <c r="F10" s="1">
@@ -3916,7 +3908,7 @@
       <c r="D11" s="1">
         <v>565.10400000000004</v>
       </c>
-      <c r="E11" s="10">
+      <c r="E11" s="9">
         <v>547.35</v>
       </c>
       <c r="F11" s="1">
@@ -3958,7 +3950,7 @@
       <c r="D12" s="1">
         <v>565.10400000000004</v>
       </c>
-      <c r="E12" s="10">
+      <c r="E12" s="9">
         <v>547.32000000000005</v>
       </c>
       <c r="F12" s="1">

</xml_diff>